<commit_message>
Added script to analyze qPCR data
</commit_message>
<xml_diff>
--- a/data/phe_growth/qPCR/Kasper_2025-07-28 14-45-16_BR005661 -  Quantification Cq Results.xlsx
+++ b/data/phe_growth/qPCR/Kasper_2025-07-28 14-45-16_BR005661 -  Quantification Cq Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasperstorck/Documents/01 IRTLab/00 Colabs-repo/data/phe_growth/qPCR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD79CF81-783C-7944-A675-40642E26478E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8C3592-5831-1244-9EBB-8493038860A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,42 +326,6 @@
     <t xml:space="preserve">3.1.1517.0823. </t>
   </si>
   <si>
-    <t>KS8-od1-1</t>
-  </si>
-  <si>
-    <t>KS8-od1-2</t>
-  </si>
-  <si>
-    <t>KS8-od1-3</t>
-  </si>
-  <si>
-    <t>KS8-od2-1</t>
-  </si>
-  <si>
-    <t>KS8-od2-2</t>
-  </si>
-  <si>
-    <t>KS8-od2-3</t>
-  </si>
-  <si>
-    <t>EHC-od1-1</t>
-  </si>
-  <si>
-    <t>EHC-od1-2</t>
-  </si>
-  <si>
-    <t>EHC-od1-3</t>
-  </si>
-  <si>
-    <t>EHC-od2-1</t>
-  </si>
-  <si>
-    <t>EHC-od2-2</t>
-  </si>
-  <si>
-    <t>EHC-od2-3</t>
-  </si>
-  <si>
     <t>EHC-1-1</t>
   </si>
   <si>
@@ -488,22 +452,58 @@
     <t>NC-2-3</t>
   </si>
   <si>
-    <t>NC-samp1-1</t>
-  </si>
-  <si>
-    <t>NC-samp1-3</t>
-  </si>
-  <si>
-    <t>NC-samp2-1</t>
-  </si>
-  <si>
-    <t>NC-samp2-2</t>
-  </si>
-  <si>
-    <t>NC-samp2-3</t>
-  </si>
-  <si>
-    <t>NC-samp1-2</t>
+    <t>KS8-od-1-1</t>
+  </si>
+  <si>
+    <t>KS8-od-1-2</t>
+  </si>
+  <si>
+    <t>KS8-od-1-3</t>
+  </si>
+  <si>
+    <t>KS8-od-2-2</t>
+  </si>
+  <si>
+    <t>KS8-od-2-3</t>
+  </si>
+  <si>
+    <t>KS8-od-2-1</t>
+  </si>
+  <si>
+    <t>EHC-od-1-1</t>
+  </si>
+  <si>
+    <t>EHC-od-1-2</t>
+  </si>
+  <si>
+    <t>EHC-od-1-3</t>
+  </si>
+  <si>
+    <t>EHC-od-2-1</t>
+  </si>
+  <si>
+    <t>EHC-od-2-2</t>
+  </si>
+  <si>
+    <t>EHC-od-2-3</t>
+  </si>
+  <si>
+    <t>NC-samp-1-1</t>
+  </si>
+  <si>
+    <t>NC-samp-1-2</t>
+  </si>
+  <si>
+    <t>NC-samp-1-3</t>
+  </si>
+  <si>
+    <t>NC-samp-2-1</t>
+  </si>
+  <si>
+    <t>NC-samp-2-2</t>
+  </si>
+  <si>
+    <t>NC-samp-2-3</t>
   </si>
 </sst>
 </file>
@@ -1038,11 +1038,11 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1128,7 +1128,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>17</v>
@@ -1166,7 +1166,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1204,7 +1204,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>17</v>
@@ -1242,7 +1242,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>17</v>
@@ -1280,7 +1280,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>17</v>
@@ -1318,7 +1318,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>17</v>
@@ -1356,7 +1356,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>17</v>
@@ -1394,7 +1394,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>17</v>
@@ -1432,7 +1432,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>17</v>
@@ -1470,7 +1470,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>17</v>
@@ -1508,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>17</v>
@@ -1546,7 +1546,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>17</v>
@@ -1584,7 +1584,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>17</v>
@@ -1622,7 +1622,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>17</v>
@@ -1660,7 +1660,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>17</v>
@@ -1698,7 +1698,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>17</v>
@@ -1736,7 +1736,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>17</v>
@@ -1774,7 +1774,7 @@
         <v>18</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>17</v>
@@ -1812,7 +1812,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>17</v>
@@ -1850,7 +1850,7 @@
         <v>18</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>17</v>
@@ -1888,7 +1888,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>17</v>
@@ -1926,7 +1926,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>17</v>
@@ -1964,7 +1964,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>17</v>
@@ -2002,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>17</v>
@@ -2040,7 +2040,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>17</v>
@@ -2078,7 +2078,7 @@
         <v>18</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>17</v>
@@ -2116,7 +2116,7 @@
         <v>18</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>17</v>
@@ -2154,7 +2154,7 @@
         <v>18</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>17</v>
@@ -2192,7 +2192,7 @@
         <v>18</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>17</v>
@@ -2230,7 +2230,7 @@
         <v>18</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>17</v>
@@ -2268,7 +2268,7 @@
         <v>18</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>17</v>
@@ -2306,7 +2306,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>17</v>
@@ -2344,7 +2344,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>17</v>
@@ -2382,7 +2382,7 @@
         <v>18</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>17</v>
@@ -2420,7 +2420,7 @@
         <v>18</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>17</v>
@@ -2458,7 +2458,7 @@
         <v>18</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>17</v>
@@ -2496,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>17</v>
@@ -2534,7 +2534,7 @@
         <v>18</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>17</v>
@@ -2572,7 +2572,7 @@
         <v>18</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>17</v>
@@ -2610,7 +2610,7 @@
         <v>18</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>17</v>
@@ -2648,7 +2648,7 @@
         <v>18</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>17</v>
@@ -2686,7 +2686,7 @@
         <v>18</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>17</v>
@@ -2724,7 +2724,7 @@
         <v>18</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>17</v>
@@ -2762,7 +2762,7 @@
         <v>18</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>17</v>
@@ -2800,7 +2800,7 @@
         <v>18</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>17</v>
@@ -2838,7 +2838,7 @@
         <v>18</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>17</v>
@@ -2876,7 +2876,7 @@
         <v>18</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>17</v>
@@ -2914,7 +2914,7 @@
         <v>18</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>17</v>
@@ -2990,7 +2990,7 @@
         <v>18</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>17</v>
@@ -3028,7 +3028,7 @@
         <v>18</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>17</v>
@@ -3066,7 +3066,7 @@
         <v>18</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>17</v>
@@ -3104,7 +3104,7 @@
         <v>18</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>17</v>
@@ -3142,7 +3142,7 @@
         <v>18</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>17</v>
@@ -3180,7 +3180,7 @@
         <v>73</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>17</v>
@@ -3218,7 +3218,7 @@
         <v>73</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>17</v>
@@ -3256,7 +3256,7 @@
         <v>73</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>17</v>
@@ -3294,7 +3294,7 @@
         <v>73</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>17</v>
@@ -3332,7 +3332,7 @@
         <v>73</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>17</v>
@@ -3370,7 +3370,7 @@
         <v>73</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>17</v>

</xml_diff>